<commit_message>
all cases of cmdf_
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_Demo_CPX_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_Demo_CPX_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda_testcases\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008F855-22E5-4579-9CD1-2B69225A5BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7232E4A6-D438-4AE3-B49F-16885AE38996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVA" sheetId="18" r:id="rId1"/>
@@ -652,7 +652,7 @@
   <dimension ref="B6:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -720,8 +720,8 @@
         <v>2005</v>
       </c>
       <c r="E8" t="str">
-        <f>"*"&amp;1/30/J8</f>
-        <v>*0.0366218893267774</v>
+        <f>"*"&amp;1/30/AVERAGE($J$8:$J$37)</f>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
@@ -748,8 +748,8 @@
         <v>2004</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ref="E9:E37" si="0">"*"&amp;1/30/J9</f>
-        <v>*0.0371029148358715</v>
+        <f t="shared" ref="E9:E37" si="0">"*"&amp;1/30/AVERAGE($J$8:$J$37)</f>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G9" t="s">
         <v>16</v>
@@ -777,7 +777,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0376582778827428</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G10" t="s">
         <v>16</v>
@@ -805,7 +805,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0383006848737176</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -833,7 +833,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0390453857988332</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -861,7 +861,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0399107949839804</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
@@ -889,7 +889,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0409192963652827</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
@@ -917,7 +917,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>*0.042098298300308</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
@@ -945,7 +945,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0434816294081404</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
@@ -973,7 +973,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0451114056914913</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0470405566751023</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G18" t="s">
         <v>16</v>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0493362847133924</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G19" t="s">
         <v>16</v>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0520848634527801</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G20" t="s">
         <v>16</v>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0553983856896693</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G21" t="s">
         <v>16</v>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0594243926015242</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G22" t="s">
         <v>16</v>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>*0.064359832122125</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G23" t="s">
         <v>16</v>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>*0.0704716368238487</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G24" t="s">
         <v>16</v>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>*0.07812761605261</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G25" t="s">
         <v>16</v>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>*0.087843748693875</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G26" t="s">
         <v>16</v>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>*0.100358130826821</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G27" t="s">
         <v>16</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>*0.116749277825501</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G28" t="s">
         <v>16</v>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>*0.138630138955377</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G29" t="s">
         <v>16</v>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>*0.168474967213957</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G30" t="s">
         <v>16</v>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>*0.210186390770337</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G31" t="s">
         <v>16</v>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>*0.270111095760195</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>*0.358923451932994</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G33" t="s">
         <v>16</v>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>*0.495254155142161</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G34" t="s">
         <v>16</v>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>*0.712977373694643</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G35" t="s">
         <v>16</v>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>*1.07652711433093</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G36" t="s">
         <v>16</v>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>*1.71473864695628</v>
+        <v>*0.0669161219926864</v>
       </c>
       <c r="G37" t="s">
         <v>16</v>

</xml_diff>